<commit_message>
Added colors and removed test values
</commit_message>
<xml_diff>
--- a/Purchasing_Tool.xlsx
+++ b/Purchasing_Tool.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfbe2e1b6c8ea94a/Documents/Axis_and_Allies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\PycharmProjects\AxisAndAllies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2329B530-4B21-4266-A1D2-814E1F0AFADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E926CA6-0D1D-4950-AFAF-427613360EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="1800" windowWidth="21600" windowHeight="11295" xr2:uid="{372CD335-5756-4194-8FA9-D84000FAD0B8}"/>
+    <workbookView xWindow="4320" yWindow="1770" windowWidth="21600" windowHeight="11295" xr2:uid="{372CD335-5756-4194-8FA9-D84000FAD0B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,15 +128,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -144,13 +150,162 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,7 +643,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,301 +653,295 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I1">
-        <v>70</v>
-      </c>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="7"/>
+      <c r="H2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="13">
+        <f>SUMPRODUCT(B2:B15, F2:F15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2">
-        <f>SUMPRODUCT(B2:B15, F2:F15)</f>
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="H3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="15">
+        <f>I1-I2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="9">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3">
-        <f>I1-I2</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
+      <c r="C15" s="9">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="D15" s="9">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>12</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>20</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>16</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <v>6</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <v>7</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
+      <c r="E15" s="9">
+        <v>2</v>
+      </c>
+      <c r="F15" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated colors on Purchasing Tool and removed test values
</commit_message>
<xml_diff>
--- a/Purchasing_Tool.xlsx
+++ b/Purchasing_Tool.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfbe2e1b6c8ea94a/Documents/Axis_and_Allies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\PycharmProjects\AxisAndAllies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2329B530-4B21-4266-A1D2-814E1F0AFADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E26B65-9BEA-4B3A-8389-13F28DE94323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="1800" windowWidth="21600" windowHeight="11295" xr2:uid="{372CD335-5756-4194-8FA9-D84000FAD0B8}"/>
+    <workbookView xWindow="4665" yWindow="2115" windowWidth="21600" windowHeight="11295" xr2:uid="{372CD335-5756-4194-8FA9-D84000FAD0B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,15 +128,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -144,13 +150,162 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,7 +643,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,301 +653,295 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I1">
-        <v>70</v>
-      </c>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="7"/>
+      <c r="H2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="13">
+        <f>SUMPRODUCT(B2:B15, F2:F15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2">
-        <f>SUMPRODUCT(B2:B15, F2:F15)</f>
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="H3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="15">
+        <f>I1-I2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="9">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3">
-        <f>I1-I2</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
+      <c r="C15" s="9">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="D15" s="9">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>12</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>20</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>16</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <v>6</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <v>7</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
+      <c r="E15" s="9">
+        <v>2</v>
+      </c>
+      <c r="F15" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>